<commit_message>
Se realizaron algunos cambios y se hizo un excel para las tareas
</commit_message>
<xml_diff>
--- a/Presentaciones/Tareas de arreglos.xlsx
+++ b/Presentaciones/Tareas de arreglos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\Documents\proyectosdegit\Clasesdec\Clases_De_C\Presentaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1B6419-3004-41B2-8C87-BCB0DD225856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0743B203-0BBF-4A78-86AD-DD954FA28A7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{30C172CD-CC3B-45A8-AEC1-E60A97A47F18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{30C172CD-CC3B-45A8-AEC1-E60A97A47F18}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1382,7 +1382,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Pseudocodigo:</a:t>
+            <a:t>Pseudocodigo: Para invertir el arreglo</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1561,8 +1561,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-MX" sz="1100"/>
-            <a:t>Pseudocodigo:</a:t>
-          </a:r>
+            <a:t>Pseudocodigo:Para</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t> contar cuantas letras tiene el arreglo</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
@@ -1593,6 +1598,81 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CuadroTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8233B839-DFA3-4138-93FB-904F2995966C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="91440"/>
+          <a:ext cx="6819900" cy="556260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100"/>
+            <a:t>Crea un programa en</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-MX" sz="1100" baseline="0"/>
+            <a:t> C que pida una cadena al usuario y muestre por pantalla la cadena invertida.</a:t>
+          </a:r>
           <a:endParaRPr lang="es-MX" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -2377,7 +2457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267A615E-ED9D-4564-9247-8D6B9BFABFB7}">
   <dimension ref="D1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
@@ -2722,7 +2802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7382D6F-8F8A-4A0E-BB53-7DBAF713FDA1}">
   <dimension ref="C5:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>

</xml_diff>